<commit_message>
experiment repetition and mean plot
</commit_message>
<xml_diff>
--- a/Comparação Resultados Fluxos.xlsx
+++ b/Comparação Resultados Fluxos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smribei\Desktop\UFMG-20180924T133728Z-001\Mestrado\Artigo\Analise de Sentimento\TimeSeriesArticle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D443BB-4DF7-412B-861E-CEBD761DB59C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90031E1-C137-4D5D-A577-5E0F74847C2E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18480" yWindow="2660" windowWidth="18160" windowHeight="10940" xr2:uid="{83A00F3E-C367-4969-88EF-98D6F3324460}"/>
+    <workbookView xWindow="2280" yWindow="2256" windowWidth="18156" windowHeight="10296" xr2:uid="{83A00F3E-C367-4969-88EF-98D6F3324460}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -200,9 +200,6 @@
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -215,6 +212,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,7 +533,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A17" sqref="A17:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,316 +547,316 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0.32173913043478197</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.32330827067669099</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.30303030303030298</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0.60244648318042804</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.66666666666666596</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>0.35087719298245601</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0.375</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.4</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.39860139860139798</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.588607594936708</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.38461538461538403</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>0.31210191082802502</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>0.41293532338308397</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>0.51750972762645897</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>0.59627329192546497</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>0.47136563876651899</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>0.60509554140127397</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>0.30645161290322498</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>0.87128712871299996</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>0.296874999999999</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>0.32800000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>0.87096774193500004</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>0.51750972762645897</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>0.59627329192546497</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>0.78301886792499997</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>0.72131147540999996</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>0.607250755287009</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>0.607250755287009</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0.60843373493975905</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>0.61309523809523803</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>0.607250755287009</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <v>0.61609907120743002</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>0.65124555160142295</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>0.61424332344213595</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>0.61194029850746201</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>0.61424332344213595</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="9">
         <v>0.689393939393939</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="8">
         <v>0.5</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>0.35714285714285698</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>0.53846153846153799</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>0.76315789473684204</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="9">
         <v>0.36538461538461497</v>
       </c>
     </row>

</xml_diff>